<commit_message>
Github link was wrong, now updated
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F04E9B9-758F-4BF3-9DA7-EC41AD469B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFDC67C-2234-49E7-9D52-9B3A765A5717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -333,7 +333,7 @@
     <t>Student Name: Javier Ramirez</t>
   </si>
   <si>
-    <t>Student Git Address: https://github.com/JaviRami2/P-P_IV_Javier_Ramirez.git</t>
+    <t>Student Git Address: https://github.com/JaviRami2/CompleteProject.git</t>
   </si>
 </sst>
 </file>
@@ -928,7 +928,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3214,7 +3214,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Rubrik updated directional and point light working and moving readme updated
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2203A700-0086-414D-A67F-1F32BEC0116B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B369BE3-EDBC-4E3B-926E-7D78FF2FB1E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,11 +1072,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1092,11 +1092,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1133,7 +1137,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1162,11 +1166,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1193,11 +1201,15 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
@@ -1205,7 +1217,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -1227,11 +1239,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>25</v>
@@ -1266,7 +1282,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
@@ -2350,11 +2366,15 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2561,11 +2581,15 @@
       <c r="D66" s="5">
         <v>1</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="E66" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G66" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>

</xml_diff>

<commit_message>
Spotlight now with motion and updated rubrik
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8789A728-B4C4-40F9-9A52-61CD3991B4CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C06FD-F82A-4A31-8668-155927C73AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1072,11 +1072,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1129,15 +1129,19 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1217,11 +1221,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1274,19 +1278,23 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -3122,7 +3130,9 @@
       <c r="C91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3142,7 +3152,9 @@
       <c r="C92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -3276,7 +3288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fixed camera(hopefully) and updated Rubrik
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C06FD-F82A-4A31-8668-155927C73AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C84592-52FF-427F-87D3-8C8512A54402}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
@@ -3288,7 +3288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated rubrik and 2 basic themes
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6196E630-B512-4B8D-928F-A4AD368D99F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495BF54A-5DCB-4B4D-AED3-D22CB41D1D3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -936,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1074,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1079,7 +1082,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1228,7 +1231,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -2969,11 +2972,15 @@
       <c r="D83" s="5">
         <v>4</v>
       </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="3"/>
+      <c r="E83" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G83" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
@@ -2990,11 +2997,15 @@
       <c r="D84" s="5">
         <v>4</v>
       </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="3"/>
+      <c r="E84" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G84" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
@@ -3136,7 +3147,9 @@
       <c r="D91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3158,7 +3171,9 @@
       <c r="D92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="3"/>
+      <c r="E92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
@@ -3291,7 +3306,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>